<commit_message>
test and tag_aparna() are now updated -- there is now an assert_equals() statement in test
</commit_message>
<xml_diff>
--- a/test2.xlsx
+++ b/test2.xlsx
@@ -505,10 +505,10 @@
     <t>emea</t>
   </si>
   <si>
-    <t>[]</t>
-  </si>
-  <si>
-    <t>['vip']</t>
+    <t>aparna</t>
+  </si>
+  <si>
+    <t>vip, aparna</t>
   </si>
 </sst>
 </file>

</xml_diff>